<commit_message>
added creation of table for primer
</commit_message>
<xml_diff>
--- a/Personal/EventDetection/Docs/paper/inventory_of_reagents_and_supplies.xlsx
+++ b/Personal/EventDetection/Docs/paper/inventory_of_reagents_and_supplies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="1240" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
   <si>
     <t>Thing</t>
   </si>
@@ -247,6 +247,24 @@
   </si>
   <si>
     <t>Freeze and Squeeze</t>
+  </si>
+  <si>
+    <t>Bio-Rad</t>
+  </si>
+  <si>
+    <t>T100</t>
+  </si>
+  <si>
+    <t>KimTech</t>
+  </si>
+  <si>
+    <t>732-6165</t>
+  </si>
+  <si>
+    <t>Protein Mods</t>
+  </si>
+  <si>
+    <t>SAVT</t>
   </si>
 </sst>
 </file>
@@ -762,7 +780,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1040,6 +1058,12 @@
       <c r="A25" t="s">
         <v>74</v>
       </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
@@ -1100,23 +1124,44 @@
       <c r="A31" t="s">
         <v>70</v>
       </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>72</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33">
+        <v>16218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34">
+        <v>5511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added better argument calling to fovea, added a simple way of batch calling scripts and getting their scores.
</commit_message>
<xml_diff>
--- a/Personal/EventDetection/Docs/paper/inventory_of_reagents_and_supplies.xlsx
+++ b/Personal/EventDetection/Docs/paper/inventory_of_reagents_and_supplies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="9840" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Thing</t>
   </si>
@@ -72,9 +72,6 @@
     <t>SPM</t>
   </si>
   <si>
-    <t>TCEP</t>
-  </si>
-  <si>
     <t>wafers</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
   </si>
   <si>
     <t>PG2-MLSL-600</t>
-  </si>
-  <si>
-    <t>Thermo Scientific</t>
   </si>
   <si>
     <t>New England BioLabs</t>
@@ -313,8 +307,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -383,7 +391,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -416,6 +424,13 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -448,6 +463,13 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -777,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -803,10 +825,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>26023</v>
@@ -814,10 +836,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>2510</v>
@@ -825,10 +847,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>2801</v>
@@ -836,13 +858,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -850,10 +872,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -861,10 +883,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -872,10 +894,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -883,285 +905,274 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16">
-        <v>28106</v>
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>28106</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20">
-        <v>14250</v>
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>14250</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="C23">
-        <v>1020</v>
+        <v>16218</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24">
-        <v>524650</v>
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>23</v>
+        <v>60</v>
+      </c>
+      <c r="C26">
+        <v>1020</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C27">
-        <v>77720</v>
+        <v>524650</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
+        <v>76</v>
+      </c>
+      <c r="C29">
+        <v>5511</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33">
-        <v>16218</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34">
-        <v>5511</v>
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed figure labelling, I hope for the last time. added in better, relative metrics. some text changes
</commit_message>
<xml_diff>
--- a/Personal/EventDetection/Docs/paper/inventory_of_reagents_and_supplies.xlsx
+++ b/Personal/EventDetection/Docs/paper/inventory_of_reagents_and_supplies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="11940" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
   <si>
     <t>Thing</t>
   </si>
@@ -259,13 +259,34 @@
   </si>
   <si>
     <t>SAVT</t>
+  </si>
+  <si>
+    <t>Sigma</t>
+  </si>
+  <si>
+    <t>Nickel</t>
+  </si>
+  <si>
+    <t>Hepes</t>
+  </si>
+  <si>
+    <t>h4034</t>
+  </si>
+  <si>
+    <t>V1 Mica</t>
+  </si>
+  <si>
+    <t>SNL-10</t>
+  </si>
+  <si>
+    <t>Bruker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -289,6 +310,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -307,7 +336,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -387,11 +416,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -431,6 +466,8 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -470,6 +507,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -799,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1034,144 +1073,188 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
+        <v>80</v>
+      </c>
+      <c r="C21">
+        <v>654507</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22">
-        <v>14250</v>
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
       </c>
-      <c r="C23">
-        <v>16218</v>
+      <c r="C23" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>57</v>
+        <v>86</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C26">
-        <v>1020</v>
+        <v>14250</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C27">
-        <v>524650</v>
+        <v>16218</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29">
-        <v>5511</v>
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" t="s">
-        <v>79</v>
+        <v>60</v>
+      </c>
+      <c r="C30">
+        <v>1020</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="s">
-        <v>59</v>
+        <v>41</v>
+      </c>
+      <c r="C31">
+        <v>524650</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33">
+        <v>5511</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>61</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>62</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C37" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>